<commit_message>
Added Day rate contractor and NMS Salary
</commit_message>
<xml_diff>
--- a/SalaryData.xlsx
+++ b/SalaryData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code Projects\CS-Meeting-Cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shoskin/Code/CS-Meeting-Cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744AD5ED-03BA-48BE-B892-559E797802FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C605426-30C2-1B46-AA33-39F77D899247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{BD2E9CBC-0550-F146-88E8-F9374378325A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16100" xr2:uid="{BD2E9CBC-0550-F146-88E8-F9374378325A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>Department</t>
   </si>
@@ -150,6 +153,54 @@
   </si>
   <si>
     <t>Band 8d</t>
+  </si>
+  <si>
+    <t>Contractor</t>
+  </si>
+  <si>
+    <t>£400 Day Rate</t>
+  </si>
+  <si>
+    <t>£500 Day Rate</t>
+  </si>
+  <si>
+    <t>£600 Day Rate</t>
+  </si>
+  <si>
+    <t>£700 Day Rate</t>
+  </si>
+  <si>
+    <t>£800 Day Rate</t>
+  </si>
+  <si>
+    <t>£900 Day Rate</t>
+  </si>
+  <si>
+    <t>£1000 Day Rate</t>
+  </si>
+  <si>
+    <t>18 to 21</t>
+  </si>
+  <si>
+    <t>22 to 29</t>
+  </si>
+  <si>
+    <t>30 to 39</t>
+  </si>
+  <si>
+    <t>40 to 49</t>
+  </si>
+  <si>
+    <t>50 to 59</t>
+  </si>
+  <si>
+    <t>60 and over</t>
+  </si>
+  <si>
+    <t>All Ages</t>
+  </si>
+  <si>
+    <t>National Medium Salary</t>
   </si>
 </sst>
 </file>
@@ -228,8 +279,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34B660D2-3985-EA41-832F-265E5E27B1BE}" name="Table1" displayName="Table1" ref="A1:H30" totalsRowShown="0">
-  <autoFilter ref="A1:H30" xr:uid="{34B660D2-3985-EA41-832F-265E5E27B1BE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34B660D2-3985-EA41-832F-265E5E27B1BE}" name="Table1" displayName="Table1" ref="A1:H44" totalsRowShown="0">
+  <autoFilter ref="A1:H44" xr:uid="{34B660D2-3985-EA41-832F-265E5E27B1BE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C17">
     <sortCondition ref="C1:C17"/>
   </sortState>
@@ -258,7 +309,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -546,7 +597,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,18 +605,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0B6CBB-E552-CE49-AC7B-E46053B78105}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +642,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -622,7 +673,7 @@
         <v>3.1361168861168865E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -653,7 +704,7 @@
         <v>3.5122141372141372E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -684,7 +735,7 @@
         <v>3.6493705243705247E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -715,7 +766,7 @@
         <v>4.0425040425040425E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -746,7 +797,7 @@
         <v>4.0497227997227997E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -777,7 +828,7 @@
         <v>4.7124047124047132E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -808,7 +859,7 @@
         <v>5.0879244629244624E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -839,7 +890,7 @@
         <v>5.492896742896743E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -870,7 +921,7 @@
         <v>5.9788634788634784E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -901,7 +952,7 @@
         <v>7.3189535689535687E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -932,7 +983,7 @@
         <v>8.0552668052668065E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -963,7 +1014,7 @@
         <v>8.9093901593901587E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -994,7 +1045,7 @@
         <v>9.498440748440749E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1025,7 +1076,7 @@
         <v>1.053938553938554E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1056,7 +1107,7 @@
         <v>1.3715638715638717E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +1138,7 @@
         <v>1.8046893046893046E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1118,7 +1169,7 @@
         <v>2.8875028875028873E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1128,28 +1179,28 @@
       <c r="C19">
         <v>20270</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>389.80769230769232</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>77.961538461538467</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>10.535343035343036</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.17558905058905061</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>2.9264841764841767E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1159,28 +1210,28 @@
       <c r="C20">
         <v>20270</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>389.80769230769232</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>77.961538461538467</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>10.535343035343036</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.17558905058905061</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>2.9264841764841767E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1190,28 +1241,28 @@
       <c r="C21">
         <v>21730</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>417.88461538461536</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>83.576923076923066</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>11.294178794178794</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.18823631323631324</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>3.1372718872718871E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1221,28 +1272,28 @@
       <c r="C22">
         <v>23949</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>460.55769230769232</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>92.111538461538458</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>12.447505197505198</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.20745841995841996</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>3.4576403326403325E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1252,28 +1303,28 @@
       <c r="C23">
         <v>27055</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>520.28846153846155</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>104.05769230769231</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>14.061850311850312</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.23436417186417188</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>3.9060695310695315E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1283,28 +1334,28 @@
       <c r="C24">
         <v>33706</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>648.19230769230774</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>129.63846153846154</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>17.51871101871102</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.29197851697851701</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>4.8663086163086167E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1314,28 +1365,28 @@
       <c r="C25">
         <v>41659</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>801.13461538461536</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>160.22692307692307</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>21.652286902286903</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.36087144837144841</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>6.0145241395241399E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1345,28 +1396,28 @@
       <c r="C26">
         <v>48526</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>933.19230769230774</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>186.63846153846154</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>25.221413721413722</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.42035689535689535</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>7.0059482559482562E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1376,28 +1427,28 @@
       <c r="C27">
         <v>56164</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>1080.0769230769231</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>216.01538461538462</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>29.191268191268193</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.48652113652113654</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>8.1086856086856098E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1407,28 +1458,28 @@
       <c r="C28">
         <v>67064</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>1289.6923076923076</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>257.93846153846152</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>34.856548856548855</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.58094248094248091</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>9.6823746823746816E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1438,28 +1489,28 @@
       <c r="C29">
         <v>79592</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>1530.6153846153845</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>306.12307692307689</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>41.367983367983364</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.68946638946638938</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>1.149110649110649E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1469,25 +1520,459 @@
       <c r="C30">
         <v>95135</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <f>Table1[[#This Row],[Salary]]/52</f>
         <v>1829.5192307692307</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30">
         <f>Table1[[#This Row],[Weekly]]/5</f>
         <v>365.90384615384613</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30">
         <f>Table1[[#This Row],[Weekly]]/37</f>
         <v>49.446465696465694</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30">
         <f>Table1[[#This Row],[Hr]]/60</f>
         <v>0.82410776160776156</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30">
         <f>Table1[[#This Row],[Min]]/60</f>
         <v>1.3735129360129359E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31">
+        <v>104000</v>
+      </c>
+      <c r="D31" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>2000</v>
+      </c>
+      <c r="E31" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>400</v>
+      </c>
+      <c r="F31" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>54.054054054054056</v>
+      </c>
+      <c r="G31" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>0.90090090090090091</v>
+      </c>
+      <c r="H31" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>1.5015015015015015E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32">
+        <v>130000</v>
+      </c>
+      <c r="D32" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>2500</v>
+      </c>
+      <c r="E32" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>500</v>
+      </c>
+      <c r="F32" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>67.567567567567565</v>
+      </c>
+      <c r="G32" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>1.1261261261261262</v>
+      </c>
+      <c r="H32" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>1.8768768768768769E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33">
+        <v>156000</v>
+      </c>
+      <c r="D33" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>3000</v>
+      </c>
+      <c r="E33" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>600</v>
+      </c>
+      <c r="F33" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>81.081081081081081</v>
+      </c>
+      <c r="G33" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>1.3513513513513513</v>
+      </c>
+      <c r="H33" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>2.2522522522522521E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34">
+        <v>182000</v>
+      </c>
+      <c r="D34" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>3500</v>
+      </c>
+      <c r="E34" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>700</v>
+      </c>
+      <c r="F34" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>94.594594594594597</v>
+      </c>
+      <c r="G34" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>1.5765765765765767</v>
+      </c>
+      <c r="H34" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>2.6276276276276277E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35">
+        <v>208000</v>
+      </c>
+      <c r="D35" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>4000</v>
+      </c>
+      <c r="E35" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>800</v>
+      </c>
+      <c r="F35" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>108.10810810810811</v>
+      </c>
+      <c r="G35" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>1.8018018018018018</v>
+      </c>
+      <c r="H35" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>3.003003003003003E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>234000</v>
+      </c>
+      <c r="D36" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>4500</v>
+      </c>
+      <c r="E36" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>900</v>
+      </c>
+      <c r="F36" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>121.62162162162163</v>
+      </c>
+      <c r="G36" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>2.0270270270270272</v>
+      </c>
+      <c r="H36" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>3.3783783783783786E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37">
+        <v>260000</v>
+      </c>
+      <c r="D37" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>5000</v>
+      </c>
+      <c r="E37" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>1000</v>
+      </c>
+      <c r="F37" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>135.13513513513513</v>
+      </c>
+      <c r="G37" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>2.2522522522522523</v>
+      </c>
+      <c r="H37" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>3.7537537537537538E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38">
+        <v>18597</v>
+      </c>
+      <c r="D38" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>357.63461538461536</v>
+      </c>
+      <c r="E38" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>71.526923076923069</v>
+      </c>
+      <c r="F38" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>9.6658004158004154</v>
+      </c>
+      <c r="G38" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>0.1610966735966736</v>
+      </c>
+      <c r="H38" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>2.6849445599445598E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39">
+        <v>27492</v>
+      </c>
+      <c r="D39" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>528.69230769230774</v>
+      </c>
+      <c r="E39" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>105.73846153846155</v>
+      </c>
+      <c r="F39" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>14.28898128898129</v>
+      </c>
+      <c r="G39" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>0.23814968814968818</v>
+      </c>
+      <c r="H39" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>3.9691614691614698E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40">
+        <v>34306</v>
+      </c>
+      <c r="D40" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>659.73076923076928</v>
+      </c>
+      <c r="E40" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>131.94615384615386</v>
+      </c>
+      <c r="F40" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>17.830561330561331</v>
+      </c>
+      <c r="G40" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>0.29717602217602218</v>
+      </c>
+      <c r="H40" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>4.9529337029337031E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41">
+        <v>36961</v>
+      </c>
+      <c r="D41" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>710.78846153846155</v>
+      </c>
+      <c r="E41" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>142.15769230769232</v>
+      </c>
+      <c r="F41" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>19.21049896049896</v>
+      </c>
+      <c r="G41" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>0.32017498267498268</v>
+      </c>
+      <c r="H41" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>5.3362497112497114E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42">
+        <v>34809</v>
+      </c>
+      <c r="D42" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>669.40384615384619</v>
+      </c>
+      <c r="E42" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>133.88076923076923</v>
+      </c>
+      <c r="F42" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>18.091995841995843</v>
+      </c>
+      <c r="G42" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>0.30153326403326403</v>
+      </c>
+      <c r="H42" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>5.0255544005544002E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43">
+        <v>30468</v>
+      </c>
+      <c r="D43" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>585.92307692307691</v>
+      </c>
+      <c r="E43" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>117.18461538461538</v>
+      </c>
+      <c r="F43" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>15.835758835758835</v>
+      </c>
+      <c r="G43" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>0.2639293139293139</v>
+      </c>
+      <c r="H43" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>4.3988218988218987E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44">
+        <v>33000</v>
+      </c>
+      <c r="D44" s="1">
+        <f>Table1[[#This Row],[Salary]]/52</f>
+        <v>634.61538461538464</v>
+      </c>
+      <c r="E44" s="1">
+        <f>Table1[[#This Row],[Weekly]]/5</f>
+        <v>126.92307692307693</v>
+      </c>
+      <c r="F44" s="1">
+        <f>Table1[[#This Row],[Weekly]]/37</f>
+        <v>17.151767151767153</v>
+      </c>
+      <c r="G44" s="1">
+        <f>Table1[[#This Row],[Hr]]/60</f>
+        <v>0.28586278586278591</v>
+      </c>
+      <c r="H44" s="1">
+        <f>Table1[[#This Row],[Min]]/60</f>
+        <v>4.7643797643797652E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added DHSC and HMT
</commit_message>
<xml_diff>
--- a/SalaryData.xlsx
+++ b/SalaryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shoskin/Code/CS-Meeting-Cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1219195B-67C1-4247-B76B-E2B00F92C116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8038DB8-AF48-D64E-8C89-A47637300A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SalaryData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="66">
   <si>
     <t>Department</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>DFIT</t>
+  </si>
+  <si>
+    <t>DHSC</t>
   </si>
 </sst>
 </file>
@@ -308,8 +311,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H90" totalsRowShown="0">
-  <autoFilter ref="A1:H90" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H97" totalsRowShown="0">
+  <autoFilter ref="A1:H97" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Department"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Grade"/>
@@ -612,10 +615,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77:H90"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90:H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3411,6 +3414,223 @@
         <v>8.931479556479556E-3</v>
       </c>
     </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>65</v>
+      </c>
+      <c r="B91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="1">
+        <v>19340</v>
+      </c>
+      <c r="D91" s="4">
+        <f>Table1[[#This Row], [Salary]]/52</f>
+        <v>371.92307692307691</v>
+      </c>
+      <c r="E91" s="4">
+        <f>Table1[[#This Row], [Weekly]]/5</f>
+        <v>74.384615384615387</v>
+      </c>
+      <c r="F91" s="4">
+        <f>Table1[[#This Row], [Weekly]]/37</f>
+        <v>10.051975051975052</v>
+      </c>
+      <c r="G91" s="4">
+        <f>Table1[[#This Row], [Hr]]/60</f>
+        <v>0.16753291753291755</v>
+      </c>
+      <c r="H91" s="4">
+        <f>Table1[[#This Row], [Min]]/60</f>
+        <v>2.7922152922152926E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>65</v>
+      </c>
+      <c r="B92" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" s="1">
+        <v>23690</v>
+      </c>
+      <c r="D92" s="4">
+        <f>Table1[[#This Row], [Salary]]/52</f>
+        <v>455.57692307692309</v>
+      </c>
+      <c r="E92" s="4">
+        <f>Table1[[#This Row], [Weekly]]/5</f>
+        <v>91.115384615384613</v>
+      </c>
+      <c r="F92" s="4">
+        <f>Table1[[#This Row], [Weekly]]/37</f>
+        <v>12.312889812889813</v>
+      </c>
+      <c r="G92" s="4">
+        <f>Table1[[#This Row], [Hr]]/60</f>
+        <v>0.2052148302148302</v>
+      </c>
+      <c r="H92" s="4">
+        <f>Table1[[#This Row], [Min]]/60</f>
+        <v>3.4202471702471701E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>65</v>
+      </c>
+      <c r="B93" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="1">
+        <v>28966</v>
+      </c>
+      <c r="D93" s="4">
+        <f>Table1[[#This Row], [Salary]]/52</f>
+        <v>557.03846153846155</v>
+      </c>
+      <c r="E93" s="4">
+        <f>Table1[[#This Row], [Weekly]]/5</f>
+        <v>111.40769230769232</v>
+      </c>
+      <c r="F93" s="4">
+        <f>Table1[[#This Row], [Weekly]]/37</f>
+        <v>15.055093555093555</v>
+      </c>
+      <c r="G93" s="4">
+        <f>Table1[[#This Row], [Hr]]/60</f>
+        <v>0.25091822591822593</v>
+      </c>
+      <c r="H93" s="4">
+        <f>Table1[[#This Row], [Min]]/60</f>
+        <v>4.1819704319704326E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>65</v>
+      </c>
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="1">
+        <v>29521</v>
+      </c>
+      <c r="D94" s="4">
+        <f>Table1[[#This Row], [Salary]]/52</f>
+        <v>567.71153846153845</v>
+      </c>
+      <c r="E94" s="4">
+        <f>Table1[[#This Row], [Weekly]]/5</f>
+        <v>113.54230769230769</v>
+      </c>
+      <c r="F94" s="4">
+        <f>Table1[[#This Row], [Weekly]]/37</f>
+        <v>15.343555093555093</v>
+      </c>
+      <c r="G94" s="4">
+        <f>Table1[[#This Row], [Hr]]/60</f>
+        <v>0.25572591822591823</v>
+      </c>
+      <c r="H94" s="4">
+        <f>Table1[[#This Row], [Min]]/60</f>
+        <v>4.2620986370986375E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>65</v>
+      </c>
+      <c r="B95" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="1">
+        <v>36819</v>
+      </c>
+      <c r="D95" s="4">
+        <f>Table1[[#This Row], [Salary]]/52</f>
+        <v>708.05769230769226</v>
+      </c>
+      <c r="E95" s="4">
+        <f>Table1[[#This Row], [Weekly]]/5</f>
+        <v>141.61153846153846</v>
+      </c>
+      <c r="F95" s="4">
+        <f>Table1[[#This Row], [Weekly]]/37</f>
+        <v>19.136694386694387</v>
+      </c>
+      <c r="G95" s="4">
+        <f>Table1[[#This Row], [Hr]]/60</f>
+        <v>0.31894490644490647</v>
+      </c>
+      <c r="H95" s="4">
+        <f>Table1[[#This Row], [Min]]/60</f>
+        <v>5.3157484407484416E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>65</v>
+      </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" s="1">
+        <v>49529</v>
+      </c>
+      <c r="D96" s="4">
+        <f>Table1[[#This Row], [Salary]]/52</f>
+        <v>952.48076923076928</v>
+      </c>
+      <c r="E96" s="4">
+        <f>Table1[[#This Row], [Weekly]]/5</f>
+        <v>190.49615384615385</v>
+      </c>
+      <c r="F96" s="4">
+        <f>Table1[[#This Row], [Weekly]]/37</f>
+        <v>25.742723492723496</v>
+      </c>
+      <c r="G96" s="4">
+        <f>Table1[[#This Row], [Hr]]/60</f>
+        <v>0.42904539154539162</v>
+      </c>
+      <c r="H96" s="4">
+        <f>Table1[[#This Row], [Min]]/60</f>
+        <v>7.1507565257565272E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>65</v>
+      </c>
+      <c r="B97" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" s="1">
+        <v>62404</v>
+      </c>
+      <c r="D97" s="4">
+        <f>Table1[[#This Row], [Salary]]/52</f>
+        <v>1200.0769230769231</v>
+      </c>
+      <c r="E97" s="4">
+        <f>Table1[[#This Row], [Weekly]]/5</f>
+        <v>240.01538461538462</v>
+      </c>
+      <c r="F97" s="4">
+        <f>Table1[[#This Row], [Weekly]]/37</f>
+        <v>32.434511434511435</v>
+      </c>
+      <c r="G97" s="4">
+        <f>Table1[[#This Row], [Hr]]/60</f>
+        <v>0.54057519057519055</v>
+      </c>
+      <c r="H97" s="4">
+        <f>Table1[[#This Row], [Min]]/60</f>
+        <v>9.0095865095865084E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>